<commit_message>
Updating Input for Revenue model
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDriver/TestRevenue/ActivityData_Jan22.xlsx
+++ b/src/test/resources/TestDriver/TestRevenue/ActivityData_Jan22.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arahmed\OneDrive - SS&amp;C Technologies, Inc\Desktop\Pers\TestRevenue (1)\TestRevenue\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arahmed\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C34EF33-64EC-4197-A2A9-7646FF16E3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B322C6-92EA-48E9-ACC0-7FC572B51291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InstrumentAttribute" sheetId="1" r:id="rId1"/>
+    <sheet name="xxProduct" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="40">
   <si>
     <t>PostingDate</t>
   </si>
@@ -126,13 +127,43 @@
   </si>
   <si>
     <t>SO5</t>
+  </si>
+  <si>
+    <t>ProductId</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>SSP</t>
+  </si>
+  <si>
+    <t>RevRec_Metod</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>AMOUNT</t>
+  </si>
+  <si>
+    <t>POINT_IN_TIME</t>
+  </si>
+  <si>
+    <t>USE SALES PRICE</t>
+  </si>
+  <si>
+    <t>RATABLE</t>
+  </si>
+  <si>
+    <t>SaaS Training</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,6 +185,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -204,7 +242,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -216,6 +254,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,7 +522,7 @@
   </sheetPr>
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -1608,4 +1647,127 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F0E43A4-DD5D-42C7-8E89-36A3B25AD3E6}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>